<commit_message>
link 수정 , 2018.10.27 record
</commit_message>
<xml_diff>
--- a/record/18년도_Record.xlsx
+++ b/record/18년도_Record.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jdwdu\taeu.github.io\record\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{8109AE99-D919-4089-BFC2-1A33C984E6E1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{33F3B938-4CF1-40DF-8F69-59C8619CBA86}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7500" xr2:uid="{8136DDE6-2A14-4426-AB5C-8D0CC7F241C8}"/>
   </bookViews>
@@ -1169,6 +1169,21 @@
         </r>
       </text>
     </comment>
+    <comment ref="A27" authorId="1" shapeId="0" xr:uid="{175C70AF-B6C5-446B-8568-B07DFB7D9251}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Turning Point!
+Mind changed
+</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="A28" authorId="1" shapeId="0" xr:uid="{BF9F9070-73B1-48E5-80CB-F3D4EDB64AFF}">
       <text>
         <r>
@@ -1221,7 +1236,29 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve"> + 2</t>
+          <t xml:space="preserve"> +
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>새벽</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> 2</t>
         </r>
         <r>
           <rPr>
@@ -1297,6 +1334,534 @@
             <charset val="129"/>
           </rPr>
           <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A29" authorId="1" shapeId="0" xr:uid="{606ED873-8C93-4460-987B-EC0655170B59}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>새벽</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> 3</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>시</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>기상</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">,
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>집</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>청소좀하고</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>, 4</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>시간</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>스터디</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>진행</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">, </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>아침시간</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> 3</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>시간에</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>다시</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>공부랑</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> +</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>유산소</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A30" authorId="1" shapeId="0" xr:uid="{26B18DFB-EDBE-4456-BDE3-8C6F49840807}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>7</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>시부터</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>~ 9</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t xml:space="preserve">시
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>10</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>시</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> ~ 3</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>시</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>~
+6</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>시간</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>정도는</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>잔</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>것</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>같음</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">. 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>새벽</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> 4</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>시반에</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t xml:space="preserve">기상함
 </t>
         </r>
       </text>
@@ -7555,7 +8120,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="190">
   <si>
     <t>카테고리</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -8369,6 +8934,10 @@
     <t>10월27일부터 본격적으로 시작하겠습니다.</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
+  <si>
+    <t>30(검색)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -8381,7 +8950,7 @@
     <numFmt numFmtId="179" formatCode="0.0_ "/>
     <numFmt numFmtId="180" formatCode="0.0_);[Red]\(0.0\)"/>
   </numFmts>
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -8569,8 +9138,16 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="17">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -8662,6 +9239,12 @@
         <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="4">
     <border>
@@ -8709,7 +9292,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="8">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
@@ -8734,8 +9317,11 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -9006,8 +9592,18 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="4" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="6" fillId="17" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" xfId="8" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="2" fillId="17" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="8">
+  <cellStyles count="9">
+    <cellStyle name="20% - 강조색4" xfId="8" builtinId="42"/>
     <cellStyle name="강조색2" xfId="1" builtinId="33"/>
     <cellStyle name="강조색4" xfId="2" builtinId="41"/>
     <cellStyle name="강조색5" xfId="4" builtinId="45"/>
@@ -9335,10 +9931,10 @@
   <dimension ref="A1:AF41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="28" ySplit="2" topLeftCell="AC3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="28" ySplit="2" topLeftCell="AC18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="AE1" sqref="AE1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="R15" sqref="R15"/>
+      <selection pane="bottomRight" activeCell="X30" sqref="X30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -9359,7 +9955,7 @@
     <col min="27" max="27" width="5" style="4" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="9" style="4"/>
     <col min="29" max="29" width="5.5" style="6" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="8.09765625" style="11" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="4.09765625" style="11" customWidth="1"/>
     <col min="31" max="31" width="5.8984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -9493,7 +10089,7 @@
         <v>29</v>
       </c>
       <c r="AD2" s="11" t="s">
-        <v>113</v>
+        <v>187</v>
       </c>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.4">
@@ -11118,78 +11714,78 @@
       </c>
     </row>
     <row r="27" spans="1:32" x14ac:dyDescent="0.4">
-      <c r="A27" s="63">
+      <c r="A27" s="90">
         <v>43398</v>
       </c>
-      <c r="B27" s="61" t="s">
+      <c r="B27" s="91" t="s">
         <v>44</v>
       </c>
-      <c r="C27" s="61"/>
-      <c r="D27" s="61"/>
-      <c r="E27" s="61"/>
-      <c r="F27" s="61">
+      <c r="C27" s="91"/>
+      <c r="D27" s="91"/>
+      <c r="E27" s="91"/>
+      <c r="F27" s="91">
         <v>40</v>
       </c>
-      <c r="G27" s="61">
+      <c r="G27" s="91">
         <v>5</v>
       </c>
-      <c r="H27" s="61">
+      <c r="H27" s="91">
         <f t="shared" si="7"/>
         <v>45</v>
       </c>
-      <c r="I27" s="61"/>
-      <c r="J27" s="61"/>
-      <c r="K27" s="61"/>
-      <c r="L27" s="61">
+      <c r="I27" s="91"/>
+      <c r="J27" s="91"/>
+      <c r="K27" s="91"/>
+      <c r="L27" s="91">
         <v>80</v>
       </c>
-      <c r="M27" s="61">
+      <c r="M27" s="91">
         <v>20</v>
       </c>
-      <c r="N27" s="61">
+      <c r="N27" s="91">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="O27" s="61"/>
-      <c r="P27" s="61"/>
-      <c r="Q27" s="61"/>
-      <c r="R27" s="61">
+      <c r="O27" s="91"/>
+      <c r="P27" s="91"/>
+      <c r="Q27" s="91"/>
+      <c r="R27" s="91">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="S27" s="61">
+      <c r="S27" s="91">
         <f t="shared" si="1"/>
         <v>145</v>
       </c>
-      <c r="T27" s="61">
+      <c r="T27" s="91">
         <v>120</v>
       </c>
-      <c r="U27" s="61">
+      <c r="U27" s="91">
         <v>10</v>
       </c>
-      <c r="V27" s="61">
+      <c r="V27" s="91">
         <v>30</v>
       </c>
-      <c r="W27" s="61">
+      <c r="W27" s="91">
         <f t="shared" si="5"/>
         <v>160</v>
       </c>
-      <c r="X27" s="61">
+      <c r="X27" s="91">
         <v>120</v>
       </c>
-      <c r="Y27" s="61"/>
-      <c r="Z27" s="61">
+      <c r="Y27" s="91"/>
+      <c r="Z27" s="91">
         <v>30</v>
       </c>
-      <c r="AA27" s="61">
+      <c r="AA27" s="91">
         <f t="shared" si="2"/>
         <v>150</v>
       </c>
-      <c r="AB27" s="61">
+      <c r="AB27" s="91">
         <f t="shared" si="3"/>
         <v>455</v>
       </c>
-      <c r="AC27" s="62">
+      <c r="AC27" s="92">
         <f t="shared" si="6"/>
         <v>7.583333333333333</v>
       </c>
@@ -11286,19 +11882,25 @@
       <c r="D29" s="61"/>
       <c r="E29" s="61"/>
       <c r="F29" s="61"/>
-      <c r="G29" s="61"/>
+      <c r="G29" s="61">
+        <v>25</v>
+      </c>
       <c r="H29" s="61">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="I29" s="61"/>
-      <c r="J29" s="61"/>
+      <c r="J29" s="61">
+        <v>90</v>
+      </c>
       <c r="K29" s="61"/>
       <c r="L29" s="61"/>
-      <c r="M29" s="61"/>
+      <c r="M29" s="61">
+        <v>170</v>
+      </c>
       <c r="N29" s="61">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>260</v>
       </c>
       <c r="O29" s="61"/>
       <c r="P29" s="61"/>
@@ -11309,7 +11911,7 @@
       </c>
       <c r="S29" s="61">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>285</v>
       </c>
       <c r="T29" s="61"/>
       <c r="U29" s="61"/>
@@ -11327,11 +11929,14 @@
       </c>
       <c r="AB29" s="61">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>285</v>
       </c>
       <c r="AC29" s="62">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>4.75</v>
+      </c>
+      <c r="AE29">
+        <v>30</v>
       </c>
     </row>
     <row r="30" spans="1:32" x14ac:dyDescent="0.4">
@@ -11370,12 +11975,16 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T30" s="61"/>
-      <c r="U30" s="61"/>
+      <c r="T30" s="61">
+        <v>10</v>
+      </c>
+      <c r="U30" s="61">
+        <v>10</v>
+      </c>
       <c r="V30" s="61"/>
       <c r="W30" s="61">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="X30" s="61"/>
       <c r="Y30" s="61"/>
@@ -11386,11 +11995,14 @@
       </c>
       <c r="AB30" s="61">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="AC30" s="62">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="AE30" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="31" spans="1:32" x14ac:dyDescent="0.4">
@@ -11576,11 +12188,11 @@
       </c>
       <c r="H34" s="4">
         <f>SUM(H3:H33)</f>
-        <v>593</v>
+        <v>618</v>
       </c>
       <c r="N34" s="4">
         <f>SUM(N3:N33)</f>
-        <v>4155</v>
+        <v>4415</v>
       </c>
       <c r="R34" s="4">
         <f>SUM(R3:R33)</f>
@@ -11588,7 +12200,7 @@
       </c>
       <c r="S34" s="4">
         <f t="shared" si="1"/>
-        <v>4748</v>
+        <v>5033</v>
       </c>
       <c r="W34" s="4">
         <f t="shared" si="5"/>
@@ -11600,11 +12212,11 @@
       </c>
       <c r="AB34" s="4">
         <f t="shared" si="3"/>
-        <v>10259</v>
+        <v>10544</v>
       </c>
       <c r="AC34" s="6">
         <f>SUM(AC3:AC33)/31</f>
-        <v>5.7924731182795695</v>
+        <v>5.9564516129032263</v>
       </c>
     </row>
     <row r="35" spans="1:31" x14ac:dyDescent="0.4">
@@ -11616,14 +12228,14 @@
       </c>
       <c r="H35" s="15">
         <f>H34/60</f>
-        <v>9.8833333333333329</v>
+        <v>10.3</v>
       </c>
       <c r="M35" s="37" t="s">
         <v>2</v>
       </c>
       <c r="N35" s="15">
         <f>N34/60</f>
-        <v>69.25</v>
+        <v>73.583333333333329</v>
       </c>
       <c r="Q35" s="37" t="s">
         <v>3</v>
@@ -11634,7 +12246,7 @@
       </c>
       <c r="S35" s="15">
         <f>S34/60</f>
-        <v>79.13333333333334</v>
+        <v>83.88333333333334</v>
       </c>
       <c r="Z35" s="37" t="s">
         <v>87</v>
@@ -11645,11 +12257,11 @@
       </c>
       <c r="AB35" s="4">
         <f>AB34/60</f>
-        <v>170.98333333333332</v>
+        <v>175.73333333333332</v>
       </c>
       <c r="AC35" s="15">
         <f>AB34/60</f>
-        <v>170.98333333333332</v>
+        <v>175.73333333333332</v>
       </c>
     </row>
     <row r="36" spans="1:31" x14ac:dyDescent="0.4">
@@ -11657,28 +12269,28 @@
         <v>131</v>
       </c>
       <c r="H36" s="4">
-        <f>H35/26</f>
-        <v>0.38012820512820511</v>
+        <f>H35/31</f>
+        <v>0.33225806451612905</v>
       </c>
       <c r="N36" s="4">
-        <f>N35/26</f>
-        <v>2.6634615384615383</v>
+        <f>N35/31</f>
+        <v>2.3736559139784945</v>
       </c>
       <c r="R36" s="4">
-        <f>R35/26</f>
+        <f>R35/31</f>
         <v>0</v>
       </c>
       <c r="S36" s="4">
-        <f>S35/16</f>
-        <v>4.9458333333333337</v>
+        <f>S35/31</f>
+        <v>2.7059139784946238</v>
       </c>
       <c r="AA36" s="4">
-        <f>AA35/26</f>
-        <v>3.5326923076923076</v>
+        <f>AA35/31</f>
+        <v>2.9629032258064516</v>
       </c>
       <c r="AC36" s="6">
         <f>AC34</f>
-        <v>5.7924731182795695</v>
+        <v>5.9564516129032263</v>
       </c>
       <c r="AD36" s="11">
         <f>30/26</f>
@@ -11686,7 +12298,7 @@
       </c>
       <c r="AE36">
         <f>AC36*AD36</f>
-        <v>6.6836228287841184</v>
+        <v>6.8728287841191067</v>
       </c>
     </row>
     <row r="37" spans="1:31" x14ac:dyDescent="0.4">
@@ -11718,11 +12330,11 @@
       </c>
       <c r="H38" s="4">
         <f>H36-H37</f>
-        <v>0.15623931623931622</v>
+        <v>0.10836917562724016</v>
       </c>
       <c r="N38" s="4">
         <f>N36-N37</f>
-        <v>4.0128205128204808E-2</v>
+        <v>-0.249677419354839</v>
       </c>
       <c r="R38" s="4">
         <f>R36-R37</f>
@@ -11730,15 +12342,15 @@
       </c>
       <c r="S38" s="4">
         <f>S36-S37</f>
-        <v>1.9558333333333335</v>
+        <v>-0.28408602150537643</v>
       </c>
       <c r="AA38" s="4">
         <f>AA36-AA37</f>
-        <v>0.29269230769230736</v>
+        <v>-0.27709677419354861</v>
       </c>
       <c r="AC38" s="4">
         <f>AC36-AC37</f>
-        <v>-0.79419354838709566</v>
+        <v>-0.63021505376343878</v>
       </c>
     </row>
     <row r="39" spans="1:31" x14ac:dyDescent="0.4">
@@ -11759,11 +12371,11 @@
       </c>
       <c r="C40" s="4">
         <f>AC35</f>
-        <v>170.98333333333332</v>
+        <v>175.73333333333332</v>
       </c>
       <c r="D40" s="39">
         <f>C40/B40</f>
-        <v>0.42427626137303553</v>
+        <v>0.43606286186931342</v>
       </c>
     </row>
     <row r="41" spans="1:31" x14ac:dyDescent="0.4">
@@ -19676,12 +20288,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="C9:G10"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="H12:H18"/>
-    <mergeCell ref="C13:G13"/>
     <mergeCell ref="D3:H3"/>
     <mergeCell ref="C21:G21"/>
     <mergeCell ref="D4:G7"/>
@@ -19695,6 +20301,12 @@
     <mergeCell ref="F14:G15"/>
     <mergeCell ref="E14:E19"/>
     <mergeCell ref="D20:F20"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="C9:G10"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="H12:H18"/>
+    <mergeCell ref="C13:G13"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>